<commit_message>
Realização do DML e DQL do exercício 1.4
</commit_message>
<xml_diff>
--- a/exercicios/1.4-exercicio-optus/MODELAGEM/1.4-exercicio-optus.xlsx
+++ b/exercicios/1.4-exercicio-optus/MODELAGEM/1.4-exercicio-optus.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\senai_sprint1_bd\exercicios\1.4-exercicio-optus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\senai_sprint1_bd\exercicios\1.4-exercicio-optus\MODELAGEM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FFF831F-DEF4-47AC-AAC3-0CD739A6EFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D4AF5D-7FCC-4C53-AA19-32F4712981C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -479,8 +479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="G2" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,13 +788,13 @@
         <v>45</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9" s="2">
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -835,13 +835,13 @@
         <v>75</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G10" s="2">
         <v>2</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -882,7 +882,7 @@
         <v>767</v>
       </c>
       <c r="E11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1"/>
       <c r="I11" s="1"/>

</xml_diff>